<commit_message>
KIBON-2041: excel vorlage fields for Gemeinden statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gemeinden.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gemeinden.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D0B6A9-D770-4FEE-B212-413049A9EC22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74AF451-BE2E-47C8-AE76-4785006D7CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Register 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Register 2" sheetId="2" r:id="rId2"/>
+    <sheet name="Register 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Register 2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +25,128 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+  <si>
+    <t>{gemeindenTitle}</t>
+  </si>
+  <si>
+    <t>{mandant}</t>
+  </si>
+  <si>
+    <t>{nameGemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{nameGemeinde}</t>
+  </si>
+  <si>
+    <t>{bfsNummer}</t>
+  </si>
+  <si>
+    <t>{bfsNummerTitle}</t>
+  </si>
+  <si>
+    <t>{gutscheinausgabestelle}</t>
+  </si>
+  <si>
+    <t>{gutscheinausgabestelleTitle}</t>
+  </si>
+  <si>
+    <t>{korrespondenzspracheGemeindeTitle}</t>
+  </si>
+  <si>
+    <t>{korrespondenzspracheGemeinde}</t>
+  </si>
+  <si>
+    <t>{angebotBGTitle}</t>
+  </si>
+  <si>
+    <t>{angebotBG}</t>
+  </si>
+  <si>
+    <t>{angebotTSTitle}</t>
+  </si>
+  <si>
+    <t>{angebotTS}</t>
+  </si>
+  <si>
+    <t>{startdatumBGTitle}</t>
+  </si>
+  <si>
+    <t>{startdatumBG}</t>
+  </si>
+  <si>
+    <t>{gemeindenPeriodenTitle}</t>
+  </si>
+  <si>
+    <t>{gesuchsperiodeTitle}</t>
+  </si>
+  <si>
+    <t>{gesuchsperiode}</t>
+  </si>
+  <si>
+    <t>{limitierungKitaTitle}</t>
+  </si>
+  <si>
+    <t>{limitierungKita}</t>
+  </si>
+  <si>
+    <t>{kontingentierungTitle}</t>
+  </si>
+  <si>
+    <t>{kontingentierung}</t>
+  </si>
+  <si>
+    <t>{nachfrageErfuelltTitle}</t>
+  </si>
+  <si>
+    <t>{nachfrageErfuellt}</t>
+  </si>
+  <si>
+    <t>{nachfrageAnzahlTitle}</t>
+  </si>
+  <si>
+    <t>{nachfrageAnzahl}</t>
+  </si>
+  <si>
+    <t>{nachfrageDauerTitle}</t>
+  </si>
+  <si>
+    <t>{nachfrageDauer}</t>
+  </si>
+  <si>
+    <t>{kostenlenkungAndere}</t>
+  </si>
+  <si>
+    <t>{kostenlenkungAndereTitle}</t>
+  </si>
+  <si>
+    <t>{welcheKostenlenkungsmassnahmenTitle}</t>
+  </si>
+  <si>
+    <t>{welcheKostenlenkungsmassnahmen}</t>
+  </si>
+  <si>
+    <t>{erwerbspensumZuschlagTitle}</t>
+  </si>
+  <si>
+    <t>{erwerbspensumZuschlag}</t>
+  </si>
+  <si>
+    <t>{rowGemeindenZahlenRepeat}</t>
+  </si>
+  <si>
+    <t>{rowGemeindeInfoRepeat}</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -35,19 +154,80 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -56,8 +236,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -337,25 +534,228 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97ADB9F-B7F2-409A-AE88-F2E4D15479F3}">
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="F5:F7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97ADB9F-B7F2-409A-AE88-F2E4D15479F3}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
KIBON-2041: adapt Gemeinden excel vorlage design
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gemeinden.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gemeinden.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74AF451-BE2E-47C8-AE76-4785006D7CAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1950151-B076-42AD-A6BB-343BC8C6DF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Register 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId1"/>
     <sheet name="Register 2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -185,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -221,30 +221,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -254,7 +237,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -538,7 +529,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,71 +552,71 @@
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="7" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
@@ -651,7 +642,7 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,77 +669,77 @@
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="H5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="I5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="6" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="H6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="J6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="K6" s="10" t="s">
         <v>34</v>
       </c>
       <c r="L6" s="9" t="s">

</xml_diff>

<commit_message>
KIBON-2046: left align gutscheinausgabestelle in Gemeinden statistik
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gemeinden.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gemeinden.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1950151-B076-42AD-A6BB-343BC8C6DF01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55ABE9D-9A93-48BA-8EE0-7DBAD1DCE8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -225,26 +225,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -528,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97ADB9F-B7F2-409A-AE88-F2E4D15479F3}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,50 +549,50 @@
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -604,19 +601,19 @@
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>15</v>
       </c>
       <c r="H8" t="s">
@@ -641,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,42 +666,42 @@
       <c r="A2" s="1"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="5" t="s">
         <v>33</v>
       </c>
     </row>
@@ -712,16 +709,16 @@
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -739,10 +736,10 @@
       <c r="J6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="7" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat(KIBON-2763): add spalte Status to report "Gemeinden"
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Gemeinden.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Gemeinden.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\new\ebegu\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02EDF2D-E8D6-4749-8A80-EADF213BE6D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37766289-53A3-48D7-9D26-60DDB7E5847A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Angaben pro Gemeinde" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
   <si>
     <t>{gemeindenTitle}</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>{limitierungTfo}</t>
+  </si>
+  <si>
+    <t>{gemeindeKennzahlenStatusTitle}</t>
+  </si>
+  <si>
+    <t>{gemeindeKennzahlenStatus}</t>
   </si>
 </sst>
 </file>
@@ -219,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -229,7 +235,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -519,7 +524,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F97ADB9F-B7F2-409A-AE88-F2E4D15479F3}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -546,45 +551,45 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -593,7 +598,7 @@
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -628,10 +633,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,28 +645,29 @@
     <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
@@ -675,29 +681,32 @@
         <v>19</v>
       </c>
       <c r="E5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -707,24 +716,27 @@
         <v>20</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="K6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>